<commit_message>
left for multi list and drag and drop
</commit_message>
<xml_diff>
--- a/data/gre.xlsx
+++ b/data/gre.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programing\python\ricite\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{184FE730-5171-42F3-9402-BDAD4F838040}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067F66DE-CBEF-43D5-98A7-519BF99F7F88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="1650" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="同义词" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="637">
   <si>
     <t>可怕的</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1789,6 +1789,790 @@
   </si>
   <si>
     <t>人为的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>barb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>尖锐而严厉的批评</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>barbarous</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>barefaced</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bargain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baroque</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>协议，讨价还价</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>barrage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有压倒之势的，集中的倾泻</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>barren</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不产生效果的，无效的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>barricade</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>障碍物，用障碍物阻止通过</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>barter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>以物换物</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>beguile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>欺骗</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bathetic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>平凡的，陈腐的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>befuddle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使困惑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bedeck</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>装饰，点缀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>belabor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>严厉批评，过度说明，喋喋不休</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>beleaguer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使困扰，使消沉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>belie</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>掩饰；与……对立，与……矛盾</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bellwether</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>领头人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>beneficent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>仁慈的；有益的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>benign</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无害的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>berate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>严厉指责</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>beseech</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>恳求</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>besmirch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>玷污，诽谤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bifurcate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使分成两支</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bigot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>固执己见者</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bland</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无趣的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blandishment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>甜言蜜语，讨好某人的话</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blasé</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>厌倦享乐的，腻烦的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blast</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>爆炸</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blatant</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>惹人注目的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blazon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使知名；修饰，装扮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blemish</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>缺点污点；损害，玷污；</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blight</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bliss</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>极度快乐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>枯萎；损害</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blithe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>愉快高兴的；无忧无虑的，漫不经心的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blueprint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blunder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>过失，犯错误</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blunt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使变钝；直率的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blur</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使变得不清楚；使不易理解</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">blurt </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>突然说出，冲动的说</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bluster</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>狂妄大声地说；喧闹的状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boggle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boisterous</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>喧闹的，吵闹的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bolster</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>支撑物；鼓励，使有精力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bombast</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>夸大的言辞</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bonhomie</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>温和，和蔼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>嘘，表示不满或者嘲笑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>恩惠，福利</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boorish</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>粗鲁无礼的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bootless</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无用的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bound</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>投入的，坚定的；界限</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boycott</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>联合抵制，拒绝参与</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bracing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>令人振奋的，给人带来活力的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>brake</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>刹车</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>brash</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>鲁莽的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>brassy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>厚脸皮的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bravado</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>假装勇敢；虚张声势</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bravura</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>优秀演技的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>brazen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大胆自信的面对；蛮横大胆的，厚颜无耻的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>breach</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>违背</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>brevity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>简短，简洁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bribe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bridle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>限制</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>brisk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>充满生机的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bristle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>咆哮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>brittle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>脆弱的；不热心地</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>broach</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提出讨论</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bromide</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>陈词滥调</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>brook</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>忍受，容许</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>browbeat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>惊吓</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bruit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>散播（未经证实）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>buck</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阻止反对</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>budge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>屈服，停止抵抗</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bulge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>突起</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>欺凌弱小者，恶霸</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bumptious</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>专横傲慢的，自以为是的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bungle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>失败</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>buoy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使振作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>buoyant</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>心情好的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>burlesque</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>恶搞，夸张模仿以嘲笑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>burnish</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>擦亮，磨光</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>buttress</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>为……提供证据和信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>byzantine</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>错综复杂的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cache</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>囤货，藏货</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cachet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>同意，威望，声望</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cacophony</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>刺耳的声音</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cavalier</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cajole</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>哄骗</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>calcify</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使僵化</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>calibrate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>调整</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有骑士精神的人；傲慢的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>burgeon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使迅速发展，蓬勃发展</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>书法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>callous</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无同情心的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>callow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不老练的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>calumniate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>诽谤，造谣，中伤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>camaraderie</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>友情</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>catharsis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>情绪的宣泄；释放</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>camouflage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>伪装；伪装手段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>canard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>谣传；误传</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>candor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>坦白，直率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>canon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>准则标准；真经，正典</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>因为怀疑而犹豫</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>calligraphy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bully</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2604,10 +3388,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7801F685-6901-40B1-B1A6-D8B8326B5834}">
-  <dimension ref="A1:B201"/>
+  <dimension ref="A1:C301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="K201" sqref="K201"/>
+    <sheetView tabSelected="1" topLeftCell="A266" workbookViewId="0">
+      <selection activeCell="B278" sqref="B278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2615,1321 +3399,3009 @@
     <col min="1" max="1" width="25.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>384</v>
       </c>
       <c r="B1" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>154</v>
       </c>
       <c r="B13" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>155</v>
       </c>
       <c r="B14" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>156</v>
       </c>
       <c r="B15" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>157</v>
       </c>
       <c r="B16" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>161</v>
       </c>
       <c r="B20" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>164</v>
       </c>
       <c r="B23" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>165</v>
       </c>
       <c r="B24" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>172</v>
       </c>
       <c r="B31" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>174</v>
       </c>
       <c r="B33" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>175</v>
       </c>
       <c r="B34" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>176</v>
       </c>
       <c r="B35" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>177</v>
       </c>
       <c r="B36" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>179</v>
       </c>
       <c r="B38" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>180</v>
       </c>
       <c r="B39" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>185</v>
       </c>
       <c r="B45" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>187</v>
       </c>
       <c r="B47" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>188</v>
       </c>
       <c r="B48" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>189</v>
       </c>
       <c r="B49" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>190</v>
       </c>
       <c r="B50" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>193</v>
       </c>
       <c r="B54" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>194</v>
       </c>
       <c r="B55" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>195</v>
       </c>
       <c r="B56" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>196</v>
       </c>
       <c r="B57" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>200</v>
       </c>
       <c r="B61" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>358</v>
       </c>
       <c r="B63" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>203</v>
       </c>
       <c r="B65" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>206</v>
       </c>
       <c r="B68" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>213</v>
       </c>
       <c r="B75" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>214</v>
       </c>
       <c r="B76" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>217</v>
       </c>
       <c r="B79" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>218</v>
       </c>
       <c r="B80" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>221</v>
       </c>
       <c r="B83" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>223</v>
       </c>
       <c r="B85" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>226</v>
       </c>
       <c r="B88" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>227</v>
       </c>
       <c r="B89" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>230</v>
       </c>
       <c r="B92" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>233</v>
       </c>
       <c r="B95" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>236</v>
       </c>
       <c r="B98" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>239</v>
       </c>
       <c r="B101" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C102">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>241</v>
       </c>
       <c r="B103" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C103">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>242</v>
       </c>
       <c r="B104" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C104">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C105">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>244</v>
       </c>
       <c r="B106" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C106">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C107">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>246</v>
       </c>
       <c r="B108" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C108">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>247</v>
       </c>
       <c r="B109" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C109">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>248</v>
       </c>
       <c r="B110" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>249</v>
       </c>
       <c r="B111" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C111">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C112">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>251</v>
       </c>
       <c r="B113" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C113">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C114">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C115">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C116">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C117">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C118">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>257</v>
       </c>
       <c r="B119" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C119">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>258</v>
       </c>
       <c r="B120" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C120">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C121">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>260</v>
       </c>
       <c r="B122" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C122">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C123">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>262</v>
       </c>
       <c r="B124" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C124">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>263</v>
       </c>
       <c r="B125" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C125">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C126">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C127">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C128">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>267</v>
       </c>
       <c r="B129" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C129">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>268</v>
       </c>
       <c r="B130" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C130">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>269</v>
       </c>
       <c r="B131" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C131">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C132">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C133">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C134">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>273</v>
       </c>
       <c r="B135" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C135">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>274</v>
       </c>
       <c r="B136" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C136">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>275</v>
       </c>
       <c r="B137" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C137">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>276</v>
       </c>
       <c r="B138" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C138">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>277</v>
       </c>
       <c r="B139" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C139">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>278</v>
       </c>
       <c r="B140" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C140">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C141">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>279</v>
       </c>
       <c r="B142" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C142">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>280</v>
       </c>
       <c r="B143" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C143">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C144">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>399</v>
       </c>
       <c r="B145" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C145">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>282</v>
       </c>
       <c r="B146" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C146">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C147">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>284</v>
       </c>
       <c r="B148" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C148">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C149">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C150">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>287</v>
       </c>
       <c r="B151" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C151">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>288</v>
       </c>
       <c r="B152" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C152">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>289</v>
       </c>
       <c r="B153" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C153">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>290</v>
       </c>
       <c r="B154" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C154">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>291</v>
       </c>
       <c r="B155" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C155">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>292</v>
       </c>
       <c r="B156" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C156">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C157">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>294</v>
       </c>
       <c r="B158" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C158">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>295</v>
       </c>
       <c r="B159" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C159">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C160">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>297</v>
       </c>
       <c r="B161" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C161">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C162">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>298</v>
       </c>
       <c r="B163" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C163">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C164">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>300</v>
       </c>
       <c r="B165" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C165">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C166">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>302</v>
       </c>
       <c r="B167" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C167">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>303</v>
       </c>
       <c r="B168" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C168">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>304</v>
       </c>
       <c r="B169" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C169">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>305</v>
       </c>
       <c r="B170" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C170">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>306</v>
       </c>
       <c r="B171" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C171">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C172">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C173">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>309</v>
       </c>
       <c r="B174" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C174">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C175">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C176">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>312</v>
       </c>
       <c r="B177" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C177">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>313</v>
       </c>
       <c r="B178" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C178">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>314</v>
       </c>
       <c r="B179" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C179">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>315</v>
       </c>
       <c r="B180" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C180">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C181">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C182">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>318</v>
       </c>
       <c r="B183" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C183">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>319</v>
       </c>
       <c r="B184" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C184">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>320</v>
       </c>
       <c r="B185" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C185">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>321</v>
       </c>
       <c r="B186" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C186">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>322</v>
       </c>
       <c r="B187" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C187">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>323</v>
       </c>
       <c r="B188" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C188">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>324</v>
       </c>
       <c r="B189" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C189">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>325</v>
       </c>
       <c r="B190" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C190">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>326</v>
       </c>
       <c r="B191" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C191">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>327</v>
       </c>
       <c r="B192" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C192">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>104</v>
       </c>
       <c r="B193" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C193">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>328</v>
       </c>
       <c r="B194" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C194">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>329</v>
       </c>
       <c r="B195" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C195">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>436</v>
       </c>
       <c r="B196" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C196">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>330</v>
       </c>
       <c r="B197" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C197">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>331</v>
       </c>
       <c r="B198" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C198">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C199">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C200">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>333</v>
+      </c>
+      <c r="C201">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>441</v>
+      </c>
+      <c r="B202" t="s">
+        <v>442</v>
+      </c>
+      <c r="C202">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>443</v>
+      </c>
+      <c r="C203">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>444</v>
+      </c>
+      <c r="C204">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>445</v>
+      </c>
+      <c r="B205" t="s">
+        <v>447</v>
+      </c>
+      <c r="C205">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>446</v>
+      </c>
+      <c r="C206">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>448</v>
+      </c>
+      <c r="B207" t="s">
+        <v>449</v>
+      </c>
+      <c r="C207">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>450</v>
+      </c>
+      <c r="B208" t="s">
+        <v>451</v>
+      </c>
+      <c r="C208">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>452</v>
+      </c>
+      <c r="B209" t="s">
+        <v>453</v>
+      </c>
+      <c r="C209">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>454</v>
+      </c>
+      <c r="B210" t="s">
+        <v>455</v>
+      </c>
+      <c r="C210">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>456</v>
+      </c>
+      <c r="B211" t="s">
+        <v>457</v>
+      </c>
+      <c r="C211">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>458</v>
+      </c>
+      <c r="B212" t="s">
+        <v>459</v>
+      </c>
+      <c r="C212">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>460</v>
+      </c>
+      <c r="B213" t="s">
+        <v>461</v>
+      </c>
+      <c r="C213">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>462</v>
+      </c>
+      <c r="B214" t="s">
+        <v>463</v>
+      </c>
+      <c r="C214">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>464</v>
+      </c>
+      <c r="B215" t="s">
+        <v>465</v>
+      </c>
+      <c r="C215">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>466</v>
+      </c>
+      <c r="B216" t="s">
+        <v>467</v>
+      </c>
+      <c r="C216">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>468</v>
+      </c>
+      <c r="B217" t="s">
+        <v>469</v>
+      </c>
+      <c r="C217">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>470</v>
+      </c>
+      <c r="B218" t="s">
+        <v>471</v>
+      </c>
+      <c r="C218">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>472</v>
+      </c>
+      <c r="B219" t="s">
+        <v>473</v>
+      </c>
+      <c r="C219">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>474</v>
+      </c>
+      <c r="B220" t="s">
+        <v>475</v>
+      </c>
+      <c r="C220">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>476</v>
+      </c>
+      <c r="B221" t="s">
+        <v>477</v>
+      </c>
+      <c r="C221">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>478</v>
+      </c>
+      <c r="B222" t="s">
+        <v>479</v>
+      </c>
+      <c r="C222">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>480</v>
+      </c>
+      <c r="B223" t="s">
+        <v>481</v>
+      </c>
+      <c r="C223">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>482</v>
+      </c>
+      <c r="B224" t="s">
+        <v>483</v>
+      </c>
+      <c r="C224">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A225" t="s">
+        <v>484</v>
+      </c>
+      <c r="B225" t="s">
+        <v>485</v>
+      </c>
+      <c r="C225">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A226" t="s">
+        <v>486</v>
+      </c>
+      <c r="B226" t="s">
+        <v>487</v>
+      </c>
+      <c r="C226">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A227" t="s">
+        <v>488</v>
+      </c>
+      <c r="B227" t="s">
+        <v>489</v>
+      </c>
+      <c r="C227">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A228" t="s">
+        <v>490</v>
+      </c>
+      <c r="B228" t="s">
+        <v>491</v>
+      </c>
+      <c r="C228">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>492</v>
+      </c>
+      <c r="B229" t="s">
+        <v>493</v>
+      </c>
+      <c r="C229">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>494</v>
+      </c>
+      <c r="B230" t="s">
+        <v>495</v>
+      </c>
+      <c r="C230">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A231" t="s">
+        <v>496</v>
+      </c>
+      <c r="B231" t="s">
+        <v>497</v>
+      </c>
+      <c r="C231">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
+        <v>498</v>
+      </c>
+      <c r="B232" t="s">
+        <v>499</v>
+      </c>
+      <c r="C232">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A233" t="s">
+        <v>500</v>
+      </c>
+      <c r="B233" t="s">
+        <v>503</v>
+      </c>
+      <c r="C233">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A234" t="s">
+        <v>501</v>
+      </c>
+      <c r="B234" t="s">
+        <v>502</v>
+      </c>
+      <c r="C234">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A235" t="s">
+        <v>504</v>
+      </c>
+      <c r="B235" t="s">
+        <v>505</v>
+      </c>
+      <c r="C235">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A236" t="s">
+        <v>506</v>
+      </c>
+      <c r="C236">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A237" t="s">
+        <v>507</v>
+      </c>
+      <c r="B237" t="s">
+        <v>508</v>
+      </c>
+      <c r="C237">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A238" t="s">
+        <v>509</v>
+      </c>
+      <c r="B238" t="s">
+        <v>510</v>
+      </c>
+      <c r="C238">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A239" t="s">
+        <v>511</v>
+      </c>
+      <c r="B239" t="s">
+        <v>512</v>
+      </c>
+      <c r="C239">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A240" t="s">
+        <v>513</v>
+      </c>
+      <c r="B240" t="s">
+        <v>514</v>
+      </c>
+      <c r="C240">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A241" t="s">
+        <v>515</v>
+      </c>
+      <c r="B241" t="s">
+        <v>516</v>
+      </c>
+      <c r="C241">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A242" t="s">
+        <v>517</v>
+      </c>
+      <c r="B242" t="s">
+        <v>634</v>
+      </c>
+      <c r="C242">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A243" t="s">
+        <v>518</v>
+      </c>
+      <c r="B243" t="s">
+        <v>519</v>
+      </c>
+      <c r="C243">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A244" t="s">
+        <v>520</v>
+      </c>
+      <c r="B244" t="s">
+        <v>521</v>
+      </c>
+      <c r="C244">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A245" t="s">
+        <v>522</v>
+      </c>
+      <c r="B245" t="s">
+        <v>523</v>
+      </c>
+      <c r="C245">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A246" t="s">
+        <v>524</v>
+      </c>
+      <c r="B246" t="s">
+        <v>525</v>
+      </c>
+      <c r="C246">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A247" t="s">
+        <v>526</v>
+      </c>
+      <c r="B247" t="s">
+        <v>527</v>
+      </c>
+      <c r="C247">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A248" t="s">
+        <v>528</v>
+      </c>
+      <c r="B248" t="s">
+        <v>529</v>
+      </c>
+      <c r="C248">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A249" t="s">
+        <v>530</v>
+      </c>
+      <c r="B249" t="s">
+        <v>531</v>
+      </c>
+      <c r="C249">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A250" t="s">
+        <v>532</v>
+      </c>
+      <c r="B250" t="s">
+        <v>533</v>
+      </c>
+      <c r="C250">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A251" t="s">
+        <v>534</v>
+      </c>
+      <c r="B251" t="s">
+        <v>535</v>
+      </c>
+      <c r="C251">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A252" t="s">
+        <v>536</v>
+      </c>
+      <c r="B252" t="s">
+        <v>537</v>
+      </c>
+      <c r="C252">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A253" t="s">
+        <v>538</v>
+      </c>
+      <c r="B253" t="s">
+        <v>539</v>
+      </c>
+      <c r="C253">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A254" t="s">
+        <v>540</v>
+      </c>
+      <c r="B254" t="s">
+        <v>541</v>
+      </c>
+      <c r="C254">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A255" t="s">
+        <v>542</v>
+      </c>
+      <c r="B255" t="s">
+        <v>543</v>
+      </c>
+      <c r="C255">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A256" t="s">
+        <v>544</v>
+      </c>
+      <c r="B256" t="s">
+        <v>545</v>
+      </c>
+      <c r="C256">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A257" t="s">
+        <v>546</v>
+      </c>
+      <c r="B257" t="s">
+        <v>547</v>
+      </c>
+      <c r="C257">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A258" t="s">
+        <v>548</v>
+      </c>
+      <c r="B258" t="s">
+        <v>549</v>
+      </c>
+      <c r="C258">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A259" t="s">
+        <v>550</v>
+      </c>
+      <c r="B259" t="s">
+        <v>551</v>
+      </c>
+      <c r="C259">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A260" t="s">
+        <v>552</v>
+      </c>
+      <c r="B260" t="s">
+        <v>553</v>
+      </c>
+      <c r="C260">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A261" t="s">
+        <v>554</v>
+      </c>
+      <c r="B261" t="s">
+        <v>555</v>
+      </c>
+      <c r="C261">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A262" t="s">
+        <v>556</v>
+      </c>
+      <c r="C262">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A263" t="s">
+        <v>557</v>
+      </c>
+      <c r="B263" t="s">
+        <v>558</v>
+      </c>
+      <c r="C263">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A264" t="s">
+        <v>559</v>
+      </c>
+      <c r="B264" t="s">
+        <v>560</v>
+      </c>
+      <c r="C264">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A265" t="s">
+        <v>561</v>
+      </c>
+      <c r="B265" t="s">
+        <v>562</v>
+      </c>
+      <c r="C265">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A266" t="s">
+        <v>563</v>
+      </c>
+      <c r="B266" t="s">
+        <v>564</v>
+      </c>
+      <c r="C266">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A267" t="s">
+        <v>565</v>
+      </c>
+      <c r="B267" t="s">
+        <v>566</v>
+      </c>
+      <c r="C267">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A268" t="s">
+        <v>567</v>
+      </c>
+      <c r="B268" t="s">
+        <v>568</v>
+      </c>
+      <c r="C268">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A269" t="s">
+        <v>569</v>
+      </c>
+      <c r="B269" t="s">
+        <v>570</v>
+      </c>
+      <c r="C269">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A270" t="s">
+        <v>571</v>
+      </c>
+      <c r="B270" t="s">
+        <v>572</v>
+      </c>
+      <c r="C270">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A271" t="s">
+        <v>573</v>
+      </c>
+      <c r="B271" t="s">
+        <v>574</v>
+      </c>
+      <c r="C271">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A272" t="s">
+        <v>575</v>
+      </c>
+      <c r="B272" t="s">
+        <v>576</v>
+      </c>
+      <c r="C272">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A273" t="s">
+        <v>577</v>
+      </c>
+      <c r="B273" t="s">
+        <v>578</v>
+      </c>
+      <c r="C273">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A274" t="s">
+        <v>579</v>
+      </c>
+      <c r="B274" t="s">
+        <v>580</v>
+      </c>
+      <c r="C274">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A275" t="s">
+        <v>636</v>
+      </c>
+      <c r="B275" t="s">
+        <v>581</v>
+      </c>
+      <c r="C275">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A276" t="s">
+        <v>582</v>
+      </c>
+      <c r="B276" t="s">
+        <v>583</v>
+      </c>
+      <c r="C276">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A277" t="s">
+        <v>584</v>
+      </c>
+      <c r="B277" t="s">
+        <v>585</v>
+      </c>
+      <c r="C277">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A278" t="s">
+        <v>586</v>
+      </c>
+      <c r="B278" t="s">
+        <v>587</v>
+      </c>
+      <c r="C278">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A279" t="s">
+        <v>588</v>
+      </c>
+      <c r="B279" t="s">
+        <v>589</v>
+      </c>
+      <c r="C279">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A280" t="s">
+        <v>590</v>
+      </c>
+      <c r="B280" t="s">
+        <v>591</v>
+      </c>
+      <c r="C280">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A281" t="s">
+        <v>592</v>
+      </c>
+      <c r="B281" t="s">
+        <v>593</v>
+      </c>
+      <c r="C281">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A282" t="s">
+        <v>594</v>
+      </c>
+      <c r="B282" t="s">
+        <v>595</v>
+      </c>
+      <c r="C282">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A283" t="s">
+        <v>596</v>
+      </c>
+      <c r="B283" t="s">
+        <v>597</v>
+      </c>
+      <c r="C283">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A284" t="s">
+        <v>598</v>
+      </c>
+      <c r="B284" t="s">
+        <v>599</v>
+      </c>
+      <c r="C284">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A285" t="s">
+        <v>600</v>
+      </c>
+      <c r="B285" t="s">
+        <v>601</v>
+      </c>
+      <c r="C285">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A286" t="s">
+        <v>602</v>
+      </c>
+      <c r="B286" t="s">
+        <v>603</v>
+      </c>
+      <c r="C286">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A287" t="s">
+        <v>604</v>
+      </c>
+      <c r="B287" t="s">
+        <v>611</v>
+      </c>
+      <c r="C287">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A288" t="s">
+        <v>605</v>
+      </c>
+      <c r="B288" t="s">
+        <v>606</v>
+      </c>
+      <c r="C288">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A289" t="s">
+        <v>607</v>
+      </c>
+      <c r="B289" t="s">
+        <v>608</v>
+      </c>
+      <c r="C289">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A290" t="s">
+        <v>609</v>
+      </c>
+      <c r="B290" t="s">
+        <v>610</v>
+      </c>
+      <c r="C290">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A291" t="s">
+        <v>612</v>
+      </c>
+      <c r="B291" t="s">
+        <v>613</v>
+      </c>
+      <c r="C291">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A292" t="s">
+        <v>635</v>
+      </c>
+      <c r="B292" t="s">
+        <v>614</v>
+      </c>
+      <c r="C292">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A293" t="s">
+        <v>615</v>
+      </c>
+      <c r="B293" t="s">
+        <v>616</v>
+      </c>
+      <c r="C293">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A294" t="s">
+        <v>617</v>
+      </c>
+      <c r="B294" t="s">
+        <v>618</v>
+      </c>
+      <c r="C294">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A295" t="s">
+        <v>619</v>
+      </c>
+      <c r="B295" t="s">
+        <v>620</v>
+      </c>
+      <c r="C295">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A296" t="s">
+        <v>621</v>
+      </c>
+      <c r="B296" t="s">
+        <v>622</v>
+      </c>
+      <c r="C296">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A297" t="s">
+        <v>623</v>
+      </c>
+      <c r="B297" t="s">
+        <v>624</v>
+      </c>
+      <c r="C297">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A298" t="s">
+        <v>625</v>
+      </c>
+      <c r="B298" t="s">
+        <v>626</v>
+      </c>
+      <c r="C298">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A299" t="s">
+        <v>627</v>
+      </c>
+      <c r="B299" t="s">
+        <v>628</v>
+      </c>
+      <c r="C299">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A300" t="s">
+        <v>629</v>
+      </c>
+      <c r="B300" t="s">
+        <v>630</v>
+      </c>
+      <c r="C300">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A301" t="s">
+        <v>631</v>
+      </c>
+      <c r="B301" t="s">
+        <v>632</v>
+      </c>
+      <c r="C301">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>